<commit_message>
fix: Remove images from Secured Mail templates
Remove the embedded images from the Secured Mail manifest and docket
templates to allow compatibility with openpyxl>2.5.9.
</commit_message>
<xml_diff>
--- a/spring_manifest/views/file_manifest/secure_mail_docket_template.xlsx
+++ b/spring_manifest/views/file_manifest/secure_mail_docket_template.xlsx
@@ -232,7 +232,7 @@
     <numFmt numFmtId="167" formatCode="DD\-MMM"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -285,13 +285,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="20"/>
       <color rgb="FF000000"/>
@@ -336,13 +329,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="32"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -551,7 +537,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,7 +553,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -583,7 +569,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -651,7 +637,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -703,7 +689,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -727,11 +713,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,7 +729,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -830,9 +816,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>561600</xdr:colOff>
+      <xdr:colOff>561240</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -841,8 +827,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4331880" y="1771560"/>
-          <a:ext cx="1501200" cy="666360"/>
+          <a:off x="4331160" y="1771560"/>
+          <a:ext cx="1499760" cy="666000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -850,12 +836,10 @@
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln>
-          <a:round/>
+          <a:noFill/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
@@ -909,26 +893,28 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>236160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>275760</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1105920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1000080</xdr:rowOff>
+      <xdr:rowOff>410760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
+        <xdr:cNvPr id="1" name="CustomShape 1">
+          <a:hlinkClick r:id="rId1"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9824040" y="95400"/>
-          <a:ext cx="2777400" cy="904680"/>
+          <a:off x="236160" y="85680"/>
+          <a:ext cx="869760" cy="325080"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -936,183 +922,10 @@
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent6"/>
-        </a:solidFill>
-        <a:ln w="31680">
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="ctr"/>
-        <a:p>
-          <a:pPr algn="ctr">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-GB" sz="3200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>View Table</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-GB" sz="3200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>47520</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3028320</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>971280</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1780200" y="85680"/>
-          <a:ext cx="2980800" cy="885600"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6"/>
-        </a:solidFill>
-        <a:ln w="31680">
-          <a:solidFill>
-            <a:schemeClr val="dk1">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="ctr"/>
-        <a:p>
-          <a:pPr algn="ctr">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="1" lang="en-GB" sz="3200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>SAVE</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-GB" sz="3200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>236160</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1106280</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>411120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1">
-          <a:hlinkClick r:id="rId1"/>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="236160" y="85680"/>
-          <a:ext cx="870120" cy="325440"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln>
-          <a:round/>
+          <a:noFill/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
@@ -1179,7 +992,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="10" style="0" width="1.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="254" min="17" style="0" width="1.71"/>
@@ -1439,7 +1252,7 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="false" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1453,20 +1266,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="30.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="20" style="0" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="254" min="21" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="254" min="21" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="255" min="255" style="0" width="2.85"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="256" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="256" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2393,7 +2206,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>